<commit_message>
feat: check RET type and check all values on test
</commit_message>
<xml_diff>
--- a/test/rules-tests3.xlsx
+++ b/test/rules-tests3.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\agarimo\rules\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A27044E-A579-4CDB-8486-3AB9B7B7EA55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D1477D9-9CCC-45FF-BB82-F6DF688BE3F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="6" xr2:uid="{F97B6F4B-53D9-4DB4-8257-AA2F9CB2A1CA}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="121">
   <si>
     <t>C1</t>
   </si>
@@ -682,9 +682,6 @@
   </si>
   <si>
     <t>5.3</t>
-  </si>
-  <si>
-    <t>something</t>
   </si>
 </sst>
 </file>
@@ -2463,8 +2460,8 @@
       <c r="E26" s="5">
         <v>27</v>
       </c>
-      <c r="F26" s="4" t="s">
-        <v>121</v>
+      <c r="F26" s="4">
+        <v>100</v>
       </c>
       <c r="G26" s="1"/>
     </row>

</xml_diff>